<commit_message>
Added MSI file and removed unneeded table from tagging workbook
</commit_message>
<xml_diff>
--- a/Excel_Files/DISARM_TAGGING_WORKBOOK.xlsx
+++ b/Excel_Files/DISARM_TAGGING_WORKBOOK.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/038c3b5ed3a64a24/Documents/GitHub/DISARMWordPlugIn/Excel_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F304A6D3-5F05-4634-BCB8-52D73909ADC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{1CAAF2C7-F21D-4762-8203-FC1A50EE59F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DISARM Red with IDs" sheetId="1" r:id="rId1"/>
+    <sheet name="DISARM Red with IDs" sheetId="3" r:id="rId1"/>
     <sheet name="DISARM Red no IDs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -1696,7 +1696,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1719,6 +1719,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor rgb="FF0070C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -1859,7 +1871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1904,6 +1916,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1951,30 +1969,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A2:P33">
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TA01: Plan Strategy"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TA02: Plan Objectives"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TA13: Target Audience Analysis"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TA14: Develop Narratives"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TA06: Develop Content"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TA15: Establish Social Assets"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="TA16: Establish Legitimacy"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TA05: Microtarget"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="TA07: Select Channels and Affordances"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="TA08: Conduct Pump Priming"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="TA09: Deliver Content"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="TA17: Maximize Exposure"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TA18: Drive Online Harms"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="TA10: Drive Offline Activity"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="TA11: Persist in the Information Environment"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="TA12: Assess Effectiveness"/>
-  </tableColumns>
-  <tableStyleInfo name=" DISARM Red with IDs-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2174,7 +2168,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2A99F8-F35A-49B4-A308-F98627493464}">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2182,7 +2176,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2204,7 +2198,7 @@
     <col min="17" max="17" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2281,1078 +2275,1078 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="18" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="18" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="18" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="17" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
+      <c r="J10" s="18"/>
+      <c r="K10" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="18" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3" t="s">
+      <c r="H11" s="17"/>
+      <c r="I11" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
+      <c r="J11" s="17"/>
+      <c r="K11" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="O11" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="17" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="18"/>
+      <c r="I12" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
+      <c r="J12" s="18"/>
+      <c r="K12" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" s="18" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="s">
+      <c r="H13" s="17"/>
+      <c r="I13" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="17" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="H14" s="18"/>
+      <c r="I14" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3" t="s">
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N14" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P14" s="18" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3" t="s">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" s="17" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="18"/>
+      <c r="E16" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="H16" s="18"/>
+      <c r="I16" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3" t="s">
+      <c r="N16" s="18"/>
+      <c r="O16" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="P16" s="3"/>
+      <c r="P16" s="18"/>
     </row>
     <row r="17" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="17"/>
+      <c r="E17" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3" t="s">
+      <c r="H17" s="17"/>
+      <c r="I17" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3" t="s">
+      <c r="N17" s="17"/>
+      <c r="O17" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="P17" s="3"/>
+      <c r="P17" s="17"/>
     </row>
     <row r="18" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="18"/>
+      <c r="E18" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3" t="s">
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3" t="s">
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="M18" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3" t="s">
+      <c r="N18" s="18"/>
+      <c r="O18" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="P18" s="3"/>
+      <c r="P18" s="18"/>
     </row>
     <row r="19" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3" t="s">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3" t="s">
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3" t="s">
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="P19" s="3"/>
+      <c r="P19" s="17"/>
     </row>
     <row r="20" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="18"/>
+      <c r="E20" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3" t="s">
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3" t="s">
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3" t="s">
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="P20" s="3"/>
+      <c r="P20" s="18"/>
     </row>
     <row r="21" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="17"/>
+      <c r="E21" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="s">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3" t="s">
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3" t="s">
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="P21" s="3"/>
+      <c r="P21" s="17"/>
     </row>
     <row r="22" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="18"/>
+      <c r="E22" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3" t="s">
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3" t="s">
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="P22" s="18"/>
     </row>
     <row r="23" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="17"/>
+      <c r="E23" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3" t="s">
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="P23" s="3"/>
+      <c r="P23" s="17"/>
     </row>
     <row r="24" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3" t="s">
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3" t="s">
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="P24" s="3"/>
+      <c r="P24" s="18"/>
     </row>
     <row r="25" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3" t="s">
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3" t="s">
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="P25" s="3"/>
+      <c r="P25" s="17"/>
     </row>
     <row r="26" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3" t="s">
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="P26" s="18"/>
     </row>
     <row r="27" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3" t="s">
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3" t="s">
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="P27" s="3"/>
+      <c r="P27" s="17"/>
     </row>
     <row r="28" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3" t="s">
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3" t="s">
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="P28" s="3"/>
+      <c r="P28" s="18"/>
     </row>
     <row r="29" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3" t="s">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="P29" s="3"/>
+      <c r="P29" s="17"/>
     </row>
     <row r="30" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3" t="s">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3" t="s">
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="P30" s="3"/>
+      <c r="P30" s="18"/>
     </row>
     <row r="31" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3" t="s">
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
     </row>
     <row r="32" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
     </row>
     <row r="33" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3363,9 +3357,6 @@
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -3378,7 +3369,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3399,7 +3390,7 @@
     <col min="16" max="16" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
New Version 1.3 of Red Framework: EEAS Requests Plus Major Enhancements to TA01 and TA02
</commit_message>
<xml_diff>
--- a/Excel_Files/DISARM_TAGGING_WORKBOOK.xlsx
+++ b/Excel_Files/DISARM_TAGGING_WORKBOOK.xlsx
@@ -1,28 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/038c3b5ed3a64a24/Documents/GitHub/DISARMWordPlugIn/Excel_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/038c3b5ed3a64a24/Documents/DISARM/Framework/Red Framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1CAAF2C7-F21D-4762-8203-FC1A50EE59F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{EC2ACDC3-267D-44A6-B2A5-A8C2E63A4F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1603823-6B3C-4F91-8DA3-5DE1FA2EA4AF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISARM Red with IDs" sheetId="3" r:id="rId1"/>
     <sheet name="DISARM Red no IDs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="623">
   <si>
     <t>Plan</t>
   </si>
@@ -219,9 +231,6 @@
     <t>T0057: Organise Events</t>
   </si>
   <si>
-    <t>T0128: Conceal People</t>
-  </si>
-  <si>
     <t>T0132.002: Content Focused</t>
   </si>
   <si>
@@ -399,9 +408,6 @@
     <t>T0061.001: Sell Merchandise</t>
   </si>
   <si>
-    <t>T0128.004: Launder Accounts</t>
-  </si>
-  <si>
     <t>T0133.002: Content</t>
   </si>
   <si>
@@ -438,9 +444,6 @@
     <t>T0126: Encourage Attendance at Events</t>
   </si>
   <si>
-    <t>T0128.005: Change Names of Accounts</t>
-  </si>
-  <si>
     <t>T0133.003: Awareness</t>
   </si>
   <si>
@@ -1038,9 +1041,6 @@
     <t>Organise Events</t>
   </si>
   <si>
-    <t>Conceal People</t>
-  </si>
-  <si>
     <t>Content Focused</t>
   </si>
   <si>
@@ -1215,9 +1215,6 @@
     <t>Control Information Environment through Offensive Cyberspace Operations</t>
   </si>
   <si>
-    <t>Launder Accounts</t>
-  </si>
-  <si>
     <t>Content</t>
   </si>
   <si>
@@ -1254,9 +1251,6 @@
     <t>Encourage Attendance at Events</t>
   </si>
   <si>
-    <t>Change Names of Accounts</t>
-  </si>
-  <si>
     <t>Awareness</t>
   </si>
   <si>
@@ -1669,13 +1663,253 @@
   </si>
   <si>
     <t>Bait Legitimate Influencers</t>
+  </si>
+  <si>
+    <t>T0074.001: Geopolitical Advantage</t>
+  </si>
+  <si>
+    <t>T0074.002: Domestic Political Advantage</t>
+  </si>
+  <si>
+    <t>T0074.003: Economic Advantage</t>
+  </si>
+  <si>
+    <t>T0074.004: Ideological Advantage</t>
+  </si>
+  <si>
+    <t>T0135: Undermine</t>
+  </si>
+  <si>
+    <t>T0135.001: Smear</t>
+  </si>
+  <si>
+    <t>T0135.002: Thwart</t>
+  </si>
+  <si>
+    <t>T0135.003: Subvert</t>
+  </si>
+  <si>
+    <t>T0135.004: Polarise</t>
+  </si>
+  <si>
+    <t>T0136: Cultivate Support</t>
+  </si>
+  <si>
+    <t>T0136.001: Defend Reputaton</t>
+  </si>
+  <si>
+    <t>T0136.002: Justify Action</t>
+  </si>
+  <si>
+    <t>T0136.003: Energise Supporters</t>
+  </si>
+  <si>
+    <t>T0136.004: Boost Reputation</t>
+  </si>
+  <si>
+    <t>T0136.005: Cultvate Support for Initiative</t>
+  </si>
+  <si>
+    <t>T0136.006: Cultivate Support for Ally</t>
+  </si>
+  <si>
+    <t>T0136.007: Recruit Members</t>
+  </si>
+  <si>
+    <t>T0136.008: Increase Prestige</t>
+  </si>
+  <si>
+    <t>T0137: Make Money</t>
+  </si>
+  <si>
+    <t>T0137.001: Generate Ad Revenue</t>
+  </si>
+  <si>
+    <t>T0137.002: Scam</t>
+  </si>
+  <si>
+    <t>T0137.003: Raise Funds</t>
+  </si>
+  <si>
+    <t>T0137.004: Sell Items under False Pretences</t>
+  </si>
+  <si>
+    <t>T0137.005: Extort</t>
+  </si>
+  <si>
+    <t>T0137.006: Manipulate Stocks</t>
+  </si>
+  <si>
+    <t>T0138: Motivate to Act</t>
+  </si>
+  <si>
+    <t>T0138.001: Encourage</t>
+  </si>
+  <si>
+    <t>T0138.002: Provoke</t>
+  </si>
+  <si>
+    <t>T0138.003: Compel</t>
+  </si>
+  <si>
+    <t>T0139: Dissuade from Acting</t>
+  </si>
+  <si>
+    <t>T0139.001: Discourage</t>
+  </si>
+  <si>
+    <t>T0139.002: Silence</t>
+  </si>
+  <si>
+    <t>T0139.003: Deter</t>
+  </si>
+  <si>
+    <t>T0140: Cause Harm</t>
+  </si>
+  <si>
+    <t>T0140.001: Defame</t>
+  </si>
+  <si>
+    <t>T0140.002: Intimidate</t>
+  </si>
+  <si>
+    <t>T0140.003: Spread Hate</t>
+  </si>
+  <si>
+    <t>T0128: Conceal Information Assets</t>
+  </si>
+  <si>
+    <t>T0128.005: Change Names of Information Assets</t>
+  </si>
+  <si>
+    <t>T0128.004: Launder Information Assets</t>
+  </si>
+  <si>
+    <t>Geopolitical Advantage</t>
+  </si>
+  <si>
+    <t>Domestic Political Advantage</t>
+  </si>
+  <si>
+    <t>Economic Advantage</t>
+  </si>
+  <si>
+    <t>Ideological Advantage</t>
+  </si>
+  <si>
+    <t>Undermine</t>
+  </si>
+  <si>
+    <t>Smear</t>
+  </si>
+  <si>
+    <t>Thwart</t>
+  </si>
+  <si>
+    <t>Subvert</t>
+  </si>
+  <si>
+    <t>Polarise</t>
+  </si>
+  <si>
+    <t>Cultivate Support</t>
+  </si>
+  <si>
+    <t>Defend Reputaton</t>
+  </si>
+  <si>
+    <t>Justify Action</t>
+  </si>
+  <si>
+    <t>Energise Supporters</t>
+  </si>
+  <si>
+    <t>Boost Reputation</t>
+  </si>
+  <si>
+    <t>Cultvate Support for Initiative</t>
+  </si>
+  <si>
+    <t>Cultivate Support for Ally</t>
+  </si>
+  <si>
+    <t>Recruit Members</t>
+  </si>
+  <si>
+    <t>Increase Prestige</t>
+  </si>
+  <si>
+    <t>Make Money</t>
+  </si>
+  <si>
+    <t>Generate Ad Revenue</t>
+  </si>
+  <si>
+    <t>Scam</t>
+  </si>
+  <si>
+    <t>Raise Funds</t>
+  </si>
+  <si>
+    <t>Sell Items under False Pretences</t>
+  </si>
+  <si>
+    <t>Extort</t>
+  </si>
+  <si>
+    <t>Manipulate Stocks</t>
+  </si>
+  <si>
+    <t>Motivate to Act</t>
+  </si>
+  <si>
+    <t>Encourage</t>
+  </si>
+  <si>
+    <t>Provoke</t>
+  </si>
+  <si>
+    <t>Compel</t>
+  </si>
+  <si>
+    <t>Dissuade from Acting</t>
+  </si>
+  <si>
+    <t>Discourage</t>
+  </si>
+  <si>
+    <t>Silence</t>
+  </si>
+  <si>
+    <t>Deter</t>
+  </si>
+  <si>
+    <t>Cause Harm</t>
+  </si>
+  <si>
+    <t>Defame</t>
+  </si>
+  <si>
+    <t>Intimidate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spread Hate</t>
+  </si>
+  <si>
+    <t>Conceal Information Assets</t>
+  </si>
+  <si>
+    <t>Launder Information Assets</t>
+  </si>
+  <si>
+    <t>Change Names of Information Assets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1695,8 +1929,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1731,6 +1971,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
         <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1871,7 +2116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1909,6 +2154,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1917,11 +2168,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2173,13 +2421,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -2198,33 +2446,33 @@
     <col min="17" max="17" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:16" ht="46.5" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="51">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2274,1079 +2522,1333 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:16" ht="51">
+      <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:16" ht="63.75">
+      <c r="A4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="1:16" ht="51">
+      <c r="A5" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="17" t="s">
+    </row>
+    <row r="6" spans="1:16" ht="63.75">
+      <c r="A6" s="19" t="s">
+        <v>544</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="I6" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="K6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="L6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="M6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="N6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="O6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="P6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="P6" s="18" t="s">
+    </row>
+    <row r="7" spans="1:16" ht="52.5" customHeight="1">
+      <c r="A7" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="I7" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="K7" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="L7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="M7" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="N7" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="O7" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="P7" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="17" t="s">
+    </row>
+    <row r="8" spans="1:16" ht="78" customHeight="1">
+      <c r="A8" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18" t="s">
+      <c r="C8" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="F8" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="G8" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="H8" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="I8" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="J8" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="K8" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="L8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="M8" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="N8" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="O8" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="P8" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="P8" s="18" t="s">
+    </row>
+    <row r="9" spans="1:16" ht="63.75">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="F9" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="I9" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="J9" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="K9" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="M9" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="N9" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="O9" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="P9" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="O9" s="17" t="s">
+    </row>
+    <row r="10" spans="1:16" ht="63.75">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="C10" s="14" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="E10" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="F10" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="G10" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="J10" s="14"/>
+      <c r="K10" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18" t="s">
+      <c r="L10" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18" t="s">
+      <c r="M10" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="N10" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="O10" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="P10" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="N10" s="18" t="s">
+    </row>
+    <row r="11" spans="1:16" ht="63.75">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="O10" s="18" t="s">
+      <c r="D11" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="P10" s="18" t="s">
+      <c r="E11" s="13" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17" t="s">
+      <c r="F11" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="G11" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="L11" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17" t="s">
+      <c r="M11" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17" t="s">
+      <c r="N11" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="O11" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="P11" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="N11" s="17" t="s">
+    </row>
+    <row r="12" spans="1:16" ht="63.75">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="F12" s="14" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18" t="s">
+      <c r="G12" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="J12" s="14"/>
+      <c r="K12" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="L12" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18" t="s">
+      <c r="M12" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18" t="s">
+      <c r="N12" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="O12" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="P12" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="N12" s="18" t="s">
+    </row>
+    <row r="13" spans="1:16" ht="63.75">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13" t="s">
+        <v>549</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="P12" s="18" t="s">
+      <c r="F13" s="13" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17" t="s">
+      <c r="G13" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17" t="s">
+      <c r="H13" s="13"/>
+      <c r="I13" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="M13" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17" t="s">
+      <c r="N13" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17" t="s">
+      <c r="O13" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="P13" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="N13" s="17" t="s">
+    </row>
+    <row r="14" spans="1:16" ht="51">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="O13" s="17" t="s">
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="P13" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="s">
+      <c r="G14" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18" t="s">
+      <c r="H14" s="14"/>
+      <c r="I14" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="M14" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18" t="s">
+      <c r="N14" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18" t="s">
+      <c r="O14" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="M14" s="18" t="s">
+      <c r="P14" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="N14" s="18" t="s">
+    </row>
+    <row r="15" spans="1:16" ht="51">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13" t="s">
+        <v>551</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="O14" s="18" t="s">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="P14" s="18" t="s">
+      <c r="F15" s="13" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17" t="s">
+      <c r="G15" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17" t="s">
+      <c r="H15" s="13"/>
+      <c r="I15" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="M15" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17" t="s">
+      <c r="N15" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17" t="s">
+      <c r="O15" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="M15" s="17" t="s">
+      <c r="P15" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="N15" s="17" t="s">
+    </row>
+    <row r="16" spans="1:16" ht="51">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="O15" s="17" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="P15" s="17" t="s">
+      <c r="F16" s="14" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
+      <c r="G16" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18" t="s">
+      <c r="H16" s="14"/>
+      <c r="I16" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="M16" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18" t="s">
+      <c r="N16" s="14"/>
+      <c r="O16" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18" t="s">
+      <c r="P16" s="14"/>
+    </row>
+    <row r="17" spans="1:16" ht="51">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13" t="s">
+        <v>553</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="M16" s="18" t="s">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18" t="s">
+      <c r="F17" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="P16" s="18"/>
-    </row>
-    <row r="17" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17" t="s">
+      <c r="G17" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
+      <c r="H17" s="13"/>
+      <c r="I17" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="M17" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17" t="s">
+      <c r="N17" s="13"/>
+      <c r="O17" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17" t="s">
+      <c r="P17" s="13"/>
+    </row>
+    <row r="18" spans="1:16" ht="51">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="M17" s="17" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17" t="s">
+      <c r="F18" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="P17" s="17"/>
-    </row>
-    <row r="18" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18" t="s">
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="M18" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18" t="s">
+      <c r="N18" s="14"/>
+      <c r="O18" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18" t="s">
+      <c r="P18" s="14"/>
+    </row>
+    <row r="19" spans="1:16" ht="51">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13" t="s">
+        <v>555</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="D19" s="13"/>
+      <c r="E19" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18" t="s">
+      <c r="F19" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="P18" s="18"/>
-    </row>
-    <row r="19" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17" t="s">
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17" t="s">
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17" t="s">
+      <c r="P19" s="13"/>
+    </row>
+    <row r="20" spans="1:16" ht="63.75">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17" t="s">
+      <c r="D20" s="14"/>
+      <c r="E20" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17" t="s">
+      <c r="F20" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="P19" s="17"/>
-    </row>
-    <row r="20" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18" t="s">
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18" t="s">
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18" t="s">
+      <c r="P20" s="14"/>
+    </row>
+    <row r="21" spans="1:16" ht="51">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18" t="s">
+      <c r="F21" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="P20" s="18"/>
-    </row>
-    <row r="21" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17" t="s">
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17" t="s">
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17" t="s">
+      <c r="P21" s="13"/>
+    </row>
+    <row r="22" spans="1:16" ht="51">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17" t="s">
+      <c r="D22" s="14"/>
+      <c r="E22" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17" t="s">
+      <c r="F22" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="P21" s="17"/>
-    </row>
-    <row r="22" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18" t="s">
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18" t="s">
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="P22" s="14"/>
+    </row>
+    <row r="23" spans="1:16" ht="51">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13" t="s">
+        <v>559</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18" t="s">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18" t="s">
+      <c r="F23" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="P22" s="18"/>
-    </row>
-    <row r="23" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17" t="s">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17" t="s">
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:16" ht="38.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17" t="s">
+      <c r="F24" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17" t="s">
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="P23" s="17"/>
-    </row>
-    <row r="24" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18" t="s">
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="P24" s="14"/>
+    </row>
+    <row r="25" spans="1:16" ht="38.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13" t="s">
+        <v>561</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18" t="s">
+      <c r="F25" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18" t="s">
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="P24" s="18"/>
-    </row>
-    <row r="25" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17" t="s">
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="P25" s="13"/>
+    </row>
+    <row r="26" spans="1:16" ht="38.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17" t="s">
+      <c r="F26" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17" t="s">
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="P25" s="17"/>
-    </row>
-    <row r="26" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18" t="s">
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="P26" s="14"/>
+    </row>
+    <row r="27" spans="1:16" ht="63.75">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13" t="s">
+        <v>563</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18" t="s">
+      <c r="F27" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18" t="s">
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="P26" s="18"/>
-    </row>
-    <row r="27" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17" t="s">
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="1:16" ht="38.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17" t="s">
+      <c r="F28" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17" t="s">
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="P27" s="17"/>
-    </row>
-    <row r="28" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18" t="s">
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="P28" s="14"/>
+    </row>
+    <row r="29" spans="1:16" ht="51">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13" t="s">
+        <v>565</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18" t="s">
+      <c r="F29" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18" t="s">
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="P28" s="18"/>
-    </row>
-    <row r="29" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17" t="s">
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="P29" s="13"/>
+    </row>
+    <row r="30" spans="1:16" ht="25.5">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17" t="s">
+      <c r="F30" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17" t="s">
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="P29" s="17"/>
-    </row>
-    <row r="30" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18" t="s">
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="P30" s="14"/>
+    </row>
+    <row r="31" spans="1:16" ht="38.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13" t="s">
+        <v>567</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18" t="s">
+      <c r="F31" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18" t="s">
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="P30" s="18"/>
-    </row>
-    <row r="31" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17" t="s">
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" spans="1:16" ht="63.75">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F32" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17" t="s">
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+    </row>
+    <row r="33" spans="1:16" ht="25.5">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13" t="s">
+        <v>569</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-    </row>
-    <row r="32" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-    </row>
-    <row r="33" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="1:16" ht="25.5">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+    </row>
+    <row r="35" spans="1:16" ht="25.5">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13" t="s">
+        <v>571</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+    </row>
+    <row r="36" spans="1:16" ht="38.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+    </row>
+    <row r="37" spans="1:16" ht="25.5">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13" t="s">
+        <v>573</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" spans="1:16" ht="25.5">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+    </row>
+    <row r="39" spans="1:16" ht="25.5">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13" t="s">
+        <v>575</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+    </row>
+    <row r="40" spans="1:16" ht="25.5">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+    </row>
+    <row r="41" spans="1:16" ht="25.5">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13" t="s">
+        <v>577</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+    </row>
+    <row r="42" spans="1:16" ht="25.5">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+    </row>
+    <row r="43" spans="1:16" ht="25.5">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3366,13 +3868,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -3390,869 +3892,901 @@
     <col min="16" max="16" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:16" ht="37.5" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="38.25">
       <c r="A2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="N2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:16" ht="51">
+      <c r="A3" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="N3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:16" ht="51">
+      <c r="A4" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="N4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:16" ht="38.25">
+      <c r="A5" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="O5" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="P5" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="M5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:16" ht="51">
+      <c r="A6" s="19" t="s">
+        <v>584</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="M6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:16" ht="51">
+      <c r="A7" s="19" t="s">
+        <v>585</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="M7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:16" ht="76.5">
+      <c r="A8" s="19" t="s">
+        <v>586</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:16" ht="51">
       <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="N9" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="P9" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:16" ht="51">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="63.75">
+      <c r="A11" s="7"/>
+      <c r="B11" s="13" t="s">
+        <v>587</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>410</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>416</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="3" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="51">
+      <c r="A12" s="7"/>
+      <c r="B12" s="13" t="s">
+        <v>588</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>418</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3" t="s">
-        <v>424</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="3" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="3" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="3" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="51">
       <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="13" t="s">
+        <v>589</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="3" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="3" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="4"/>
       <c r="L13" s="3" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="38.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="13" t="s">
+        <v>590</v>
+      </c>
       <c r="C14" s="3" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="3" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="3" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="5"/>
       <c r="L14" s="3" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="38.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="13" t="s">
+        <v>591</v>
+      </c>
       <c r="C15" s="3" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="3" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="3" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="5"/>
       <c r="L15" s="3" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="38.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="13" t="s">
+        <v>592</v>
+      </c>
       <c r="C16" s="3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="3" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="3" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="5"/>
       <c r="L16" s="3" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="3" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="38.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="13" t="s">
+        <v>593</v>
+      </c>
       <c r="C17" s="3" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="3" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="3" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="5"/>
       <c r="L17" s="3" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="3" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="P17" s="9"/>
     </row>
-    <row r="18" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="38.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="13" t="s">
+        <v>594</v>
+      </c>
       <c r="C18" s="3" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="3" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="5"/>
       <c r="I18" s="3" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="5"/>
       <c r="L18" s="3" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="3" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="P18" s="9"/>
     </row>
-    <row r="19" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="38.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="13" t="s">
+        <v>595</v>
+      </c>
       <c r="C19" s="3" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="3" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="5"/>
       <c r="I19" s="3" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="5"/>
       <c r="L19" s="3" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="5"/>
       <c r="O19" s="3" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="P19" s="9"/>
     </row>
-    <row r="20" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="51">
       <c r="A20" s="7"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="13" t="s">
+        <v>596</v>
+      </c>
       <c r="C20" s="3" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="11" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="5"/>
       <c r="I20" s="3" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="5"/>
       <c r="L20" s="3" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="5"/>
       <c r="O20" s="3" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="P20" s="9"/>
     </row>
-    <row r="21" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="38.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="5"/>
+      <c r="B21" s="13" t="s">
+        <v>597</v>
+      </c>
       <c r="C21" s="3" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="3" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="5"/>
       <c r="I21" s="3" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="5"/>
       <c r="L21" s="3" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="5"/>
       <c r="O21" s="3" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="P21" s="9"/>
     </row>
-    <row r="22" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="38.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="5"/>
+      <c r="B22" s="13" t="s">
+        <v>598</v>
+      </c>
       <c r="C22" s="3" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="3" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="5"/>
       <c r="I22" s="3" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="7"/>
@@ -4260,27 +4794,29 @@
       <c r="M22" s="7"/>
       <c r="N22" s="5"/>
       <c r="O22" s="3" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="P22" s="9"/>
     </row>
-    <row r="23" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="38.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="C23" s="3" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="3" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="5"/>
       <c r="I23" s="3" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="7"/>
@@ -4288,25 +4824,27 @@
       <c r="M23" s="7"/>
       <c r="N23" s="5"/>
       <c r="O23" s="3" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="38.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="13" t="s">
+        <v>600</v>
+      </c>
       <c r="C24" s="12"/>
       <c r="D24" s="5"/>
       <c r="E24" s="3" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="5"/>
       <c r="I24" s="3" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="7"/>
@@ -4314,25 +4852,27 @@
       <c r="M24" s="7"/>
       <c r="N24" s="5"/>
       <c r="O24" s="3" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="P24" s="9"/>
     </row>
-    <row r="25" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="38.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="13" t="s">
+        <v>601</v>
+      </c>
       <c r="C25" s="7"/>
       <c r="D25" s="5"/>
       <c r="E25" s="3" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="5"/>
       <c r="I25" s="3" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="7"/>
@@ -4340,25 +4880,27 @@
       <c r="M25" s="7"/>
       <c r="N25" s="5"/>
       <c r="O25" s="3" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="P25" s="9"/>
     </row>
-    <row r="26" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="38.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="13" t="s">
+        <v>602</v>
+      </c>
       <c r="C26" s="7"/>
       <c r="D26" s="5"/>
       <c r="E26" s="3" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="5"/>
       <c r="I26" s="3" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="7"/>
@@ -4366,25 +4908,27 @@
       <c r="M26" s="7"/>
       <c r="N26" s="5"/>
       <c r="O26" s="3" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="P26" s="9"/>
     </row>
-    <row r="27" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="51">
       <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="13" t="s">
+        <v>603</v>
+      </c>
       <c r="C27" s="7"/>
       <c r="D27" s="5"/>
       <c r="E27" s="3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="5"/>
       <c r="I27" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="7"/>
@@ -4392,25 +4936,27 @@
       <c r="M27" s="7"/>
       <c r="N27" s="5"/>
       <c r="O27" s="3" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="P27" s="9"/>
     </row>
-    <row r="28" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="38.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="B28" s="13" t="s">
+        <v>604</v>
+      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="5"/>
       <c r="E28" s="3" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
       <c r="I28" s="3" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="7"/>
@@ -4418,25 +4964,27 @@
       <c r="M28" s="7"/>
       <c r="N28" s="5"/>
       <c r="O28" s="3" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="P28" s="9"/>
     </row>
-    <row r="29" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="38.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="B29" s="13" t="s">
+        <v>605</v>
+      </c>
       <c r="C29" s="7"/>
       <c r="D29" s="5"/>
       <c r="E29" s="3" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="5"/>
       <c r="I29" s="3" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="7"/>
@@ -4444,25 +4992,27 @@
       <c r="M29" s="7"/>
       <c r="N29" s="5"/>
       <c r="O29" s="3" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P29" s="9"/>
     </row>
-    <row r="30" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="25.5">
       <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="13" t="s">
+        <v>606</v>
+      </c>
       <c r="C30" s="7"/>
       <c r="D30" s="5"/>
       <c r="E30" s="3" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="5"/>
       <c r="I30" s="3" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="7"/>
@@ -4470,25 +5020,27 @@
       <c r="M30" s="7"/>
       <c r="N30" s="5"/>
       <c r="O30" s="3" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="P30" s="9"/>
     </row>
-    <row r="31" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="25.5">
       <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="B31" s="13" t="s">
+        <v>607</v>
+      </c>
       <c r="C31" s="7"/>
       <c r="D31" s="5"/>
       <c r="E31" s="3" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="5"/>
       <c r="I31" s="3" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="7"/>
@@ -4498,16 +5050,18 @@
       <c r="O31" s="12"/>
       <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="51">
       <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
+      <c r="B32" s="13" t="s">
+        <v>608</v>
+      </c>
       <c r="C32" s="7"/>
       <c r="D32" s="5"/>
       <c r="E32" s="3" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="7"/>
@@ -4520,13 +5074,15 @@
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="25.5">
       <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
+      <c r="B33" s="13" t="s">
+        <v>609</v>
+      </c>
       <c r="C33" s="7"/>
       <c r="D33" s="5"/>
       <c r="E33" s="3" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="7"/>
@@ -4540,6 +5096,56 @@
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
     </row>
+    <row r="34" spans="1:16">
+      <c r="B34" s="13" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="B35" s="13" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="25.5">
+      <c r="B36" s="13" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="B37" s="13" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="B38" s="13" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="B39" s="13" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="B40" s="13" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="B41" s="13" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="B42" s="13" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="B43" s="13" t="s">
+        <v>619</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>

</xml_diff>